<commit_message>
Many tests fixed and code refactors.
</commit_message>
<xml_diff>
--- a/tests/testing_files/ref_srch_report_tabular4.xlsx
+++ b/tests/testing_files/ref_srch_report_tabular4.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparda\Desktop\Moseley Lab\Code\academic_tracker\tests\testing_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923F5A98-2779-4AC8-89B2-E3664D4E11A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1785" yWindow="765" windowWidth="25350" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="50">
   <si>
     <t>Authors</t>
   </si>
@@ -97,7 +103,10 @@
     <t>Christian D. Powell, Hunter N.B. Moseley</t>
   </si>
   <si>
-    <t>None Found</t>
+    <t>1419282</t>
+  </si>
+  <si>
+    <t>P42ES007380, R03OD030603, 1419282, 2020026</t>
   </si>
   <si>
     <t>None</t>
@@ -118,12 +127,6 @@
     <t>The mwtab Python Library for RESTful Access and Enhanced Quality Control, Deposition, and Curation of the Metabolomics Workbench Data Repository</t>
   </si>
   <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
     <t>Atom Identifiers Generated by a Neighborhood-Specific Graph Coloring Method Enable Compound Harmonization across Metabolic Databases.</t>
   </si>
   <si>
@@ -140,9 +143,6 @@
   </si>
   <si>
     <t>Powell C, Moseley H.  The mwtab Python Library for RESTful Access and Enhanced Quality Control, Deposition, and Curation of the Metabolomics Workbench Data Repository. Metabolites. 2021 March; 11(3):163-. doi: 10.3390/metabo11030163.</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Jin, Huan</t>
@@ -175,8 +175,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,13 +239,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -283,7 +291,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -317,6 +325,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -351,9 +360,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -526,14 +536,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +622,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -618,76 +630,73 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="N2">
+        <v>2020</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="W2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" t="s">
         <v>43</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -695,76 +704,73 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="N3">
+        <v>2020</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="W3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" t="s">
         <v>43</v>
       </c>
-      <c r="X3" t="s">
-        <v>45</v>
-      </c>
       <c r="Y3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -772,227 +778,218 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="N4">
+        <v>2020</v>
       </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U4" t="s">
-        <v>40</v>
-      </c>
-      <c r="V4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="W4" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" t="s">
         <v>43</v>
       </c>
-      <c r="X4" t="s">
-        <v>45</v>
-      </c>
       <c r="Y4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5">
+        <v>2021</v>
+      </c>
+      <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" t="s">
-        <v>30</v>
-      </c>
       <c r="S5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" t="s">
         <v>42</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>44</v>
       </c>
-      <c r="X5" t="s">
-        <v>46</v>
-      </c>
       <c r="Y5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6">
+        <v>2021</v>
+      </c>
+      <c r="O6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" t="s">
         <v>31</v>
       </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" t="s">
-        <v>30</v>
-      </c>
       <c r="S6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U6" t="s">
-        <v>41</v>
-      </c>
-      <c r="V6" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" t="s">
         <v>42</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>44</v>
       </c>
-      <c r="X6" t="s">
-        <v>46</v>
-      </c>
       <c r="Y6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>